<commit_message>
Resolução do erro do random. Math.abs() e modulus Correção BD
</commit_message>
<xml_diff>
--- a/SBC_Parte11/Form SBC (Respostas).xlsx
+++ b/SBC_Parte11/Form SBC (Respostas).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\OneDrive\Ambiente de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\Universidade\2º semestre\SBC\SBC_Parte11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CDF74D-224C-4ECB-A11E-70F429DF777E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C4FBF9-56B8-49AA-ABC6-57661EFF5792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respostas do Formulário 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="74">
   <si>
     <t>Regime</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>Ocasiao</t>
+  </si>
+  <si>
+    <t>Restricao</t>
+  </si>
+  <si>
+    <t>nao</t>
   </si>
 </sst>
 </file>
@@ -519,19 +525,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E999"/>
+  <dimension ref="A1:F999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E114" sqref="E114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="21.54296875" customWidth="1"/>
+    <col min="1" max="5" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,11 +550,14 @@
       <c r="D1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -561,11 +570,14 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -578,11 +590,14 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -595,11 +610,14 @@
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -612,11 +630,14 @@
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -629,11 +650,14 @@
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -646,11 +670,14 @@
       <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -663,11 +690,14 @@
       <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -680,11 +710,14 @@
       <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -697,11 +730,14 @@
       <c r="D10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -714,11 +750,14 @@
       <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -731,11 +770,14 @@
       <c r="D12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -748,11 +790,14 @@
       <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -765,11 +810,14 @@
       <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -782,11 +830,14 @@
       <c r="D15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -799,11 +850,14 @@
       <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -816,11 +870,14 @@
       <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -833,11 +890,14 @@
       <c r="D18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -850,11 +910,14 @@
       <c r="D19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -867,11 +930,14 @@
       <c r="D20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -884,11 +950,14 @@
       <c r="D21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -901,11 +970,14 @@
       <c r="D22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -918,11 +990,14 @@
       <c r="D23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
@@ -935,11 +1010,14 @@
       <c r="D24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -952,11 +1030,14 @@
       <c r="D25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -969,11 +1050,14 @@
       <c r="D26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -986,11 +1070,14 @@
       <c r="D27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -1003,11 +1090,14 @@
       <c r="D28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
@@ -1020,11 +1110,14 @@
       <c r="D29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
@@ -1037,11 +1130,14 @@
       <c r="D30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
@@ -1054,11 +1150,14 @@
       <c r="D31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -1071,11 +1170,14 @@
       <c r="D32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>22</v>
       </c>
@@ -1088,11 +1190,14 @@
       <c r="D33" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -1105,11 +1210,14 @@
       <c r="D34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
@@ -1122,11 +1230,14 @@
       <c r="D35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>22</v>
       </c>
@@ -1139,11 +1250,14 @@
       <c r="D36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -1156,11 +1270,14 @@
       <c r="D37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
@@ -1173,11 +1290,14 @@
       <c r="D38" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
@@ -1190,11 +1310,14 @@
       <c r="D39" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>22</v>
       </c>
@@ -1207,11 +1330,14 @@
       <c r="D40" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
@@ -1224,11 +1350,14 @@
       <c r="D41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>22</v>
       </c>
@@ -1241,11 +1370,14 @@
       <c r="D42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
@@ -1258,11 +1390,14 @@
       <c r="D43" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
@@ -1275,11 +1410,14 @@
       <c r="D44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>22</v>
       </c>
@@ -1292,11 +1430,14 @@
       <c r="D45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>3</v>
       </c>
@@ -1309,11 +1450,14 @@
       <c r="D46" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
@@ -1326,11 +1470,14 @@
       <c r="D47" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>22</v>
       </c>
@@ -1343,11 +1490,14 @@
       <c r="D48" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
@@ -1360,11 +1510,14 @@
       <c r="D49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -1377,11 +1530,14 @@
       <c r="D50" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -1394,11 +1550,14 @@
       <c r="D51" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>22</v>
       </c>
@@ -1411,11 +1570,14 @@
       <c r="D52" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
@@ -1428,11 +1590,14 @@
       <c r="D53" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>22</v>
       </c>
@@ -1445,11 +1610,14 @@
       <c r="D54" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
@@ -1462,11 +1630,14 @@
       <c r="D55" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>22</v>
       </c>
@@ -1479,11 +1650,14 @@
       <c r="D56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>3</v>
       </c>
@@ -1496,11 +1670,14 @@
       <c r="D57" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -1513,11 +1690,14 @@
       <c r="D58" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>22</v>
       </c>
@@ -1530,11 +1710,14 @@
       <c r="D59" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>3</v>
       </c>
@@ -1547,11 +1730,14 @@
       <c r="D60" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F60" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -1564,11 +1750,14 @@
       <c r="D61" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>3</v>
       </c>
@@ -1581,11 +1770,14 @@
       <c r="D62" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>22</v>
       </c>
@@ -1598,11 +1790,14 @@
       <c r="D63" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>3</v>
       </c>
@@ -1615,11 +1810,14 @@
       <c r="D64" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E64" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -1632,11 +1830,14 @@
       <c r="D65" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F65" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>22</v>
       </c>
@@ -1649,11 +1850,14 @@
       <c r="D66" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
@@ -1666,11 +1870,14 @@
       <c r="D67" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>3</v>
       </c>
@@ -1683,11 +1890,14 @@
       <c r="D68" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>22</v>
       </c>
@@ -1700,11 +1910,14 @@
       <c r="D69" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E69" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>7</v>
       </c>
@@ -1717,11 +1930,14 @@
       <c r="D70" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="E70" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>3</v>
       </c>
@@ -1734,11 +1950,14 @@
       <c r="D71" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E71" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F71" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>22</v>
       </c>
@@ -1751,11 +1970,14 @@
       <c r="D72" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="E72" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F72" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>3</v>
       </c>
@@ -1768,11 +1990,14 @@
       <c r="D73" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E73" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F73" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>7</v>
       </c>
@@ -1785,11 +2010,14 @@
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E74" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F74" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>22</v>
       </c>
@@ -1802,11 +2030,14 @@
       <c r="D75" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="E75" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>3</v>
       </c>
@@ -1819,11 +2050,14 @@
       <c r="D76" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="E76" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F76" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>7</v>
       </c>
@@ -1836,11 +2070,14 @@
       <c r="D77" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E77" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F77" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>3</v>
       </c>
@@ -1853,11 +2090,14 @@
       <c r="D78" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E78" s="3" t="s">
+      <c r="E78" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F78" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>22</v>
       </c>
@@ -1870,11 +2110,14 @@
       <c r="D79" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E79" s="3" t="s">
+      <c r="E79" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F79" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>3</v>
       </c>
@@ -1887,11 +2130,14 @@
       <c r="D80" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E80" s="3" t="s">
+      <c r="E80" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F80" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>22</v>
       </c>
@@ -1904,11 +2150,14 @@
       <c r="D81" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E81" s="3" t="s">
+      <c r="E81" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F81" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>7</v>
       </c>
@@ -1921,11 +2170,14 @@
       <c r="D82" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="E82" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F82" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>3</v>
       </c>
@@ -1938,11 +2190,14 @@
       <c r="D83" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E83" s="3" t="s">
+      <c r="E83" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F83" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>22</v>
       </c>
@@ -1955,11 +2210,14 @@
       <c r="D84" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="E84" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F84" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>7</v>
       </c>
@@ -1972,11 +2230,14 @@
       <c r="D85" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E85" s="3" t="s">
+      <c r="E85" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F85" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>22</v>
       </c>
@@ -1989,11 +2250,14 @@
       <c r="D86" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E86" s="3" t="s">
+      <c r="E86" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F86" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>3</v>
       </c>
@@ -2006,11 +2270,14 @@
       <c r="D87" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E87" s="3" t="s">
+      <c r="E87" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F87" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>22</v>
       </c>
@@ -2023,11 +2290,14 @@
       <c r="D88" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E88" s="3" t="s">
+      <c r="E88" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F88" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>7</v>
       </c>
@@ -2040,11 +2310,14 @@
       <c r="D89" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E89" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F89" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>3</v>
       </c>
@@ -2057,11 +2330,14 @@
       <c r="D90" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E90" s="3" t="s">
+      <c r="E90" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F90" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>7</v>
       </c>
@@ -2074,11 +2350,14 @@
       <c r="D91" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E91" s="3" t="s">
+      <c r="E91" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F91" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>22</v>
       </c>
@@ -2091,11 +2370,14 @@
       <c r="D92" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E92" s="3" t="s">
+      <c r="E92" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F92" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>3</v>
       </c>
@@ -2108,11 +2390,14 @@
       <c r="D93" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E93" s="3" t="s">
+      <c r="E93" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F93" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>7</v>
       </c>
@@ -2125,11 +2410,14 @@
       <c r="D94" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E94" s="3" t="s">
+      <c r="E94" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F94" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>3</v>
       </c>
@@ -2142,11 +2430,14 @@
       <c r="D95" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="E95" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F95" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>22</v>
       </c>
@@ -2159,11 +2450,14 @@
       <c r="D96" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="E96" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F96" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>7</v>
       </c>
@@ -2176,11 +2470,14 @@
       <c r="D97" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E97" s="3" t="s">
+      <c r="E97" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F97" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>3</v>
       </c>
@@ -2193,11 +2490,14 @@
       <c r="D98" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="E98" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F98" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>22</v>
       </c>
@@ -2210,11 +2510,14 @@
       <c r="D99" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E99" s="3" t="s">
+      <c r="E99" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F99" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>7</v>
       </c>
@@ -2227,11 +2530,14 @@
       <c r="D100" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E100" s="3" t="s">
+      <c r="E100" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F100" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>3</v>
       </c>
@@ -2244,11 +2550,14 @@
       <c r="D101" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E101" s="3" t="s">
+      <c r="E101" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F101" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>3</v>
       </c>
@@ -2261,11 +2570,14 @@
       <c r="D102" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E102" s="3" t="s">
+      <c r="E102" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F102" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>3</v>
       </c>
@@ -2278,11 +2590,14 @@
       <c r="D103" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="E103" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F103" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>3</v>
       </c>
@@ -2295,11 +2610,14 @@
       <c r="D104" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="E104" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F104" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>3</v>
       </c>
@@ -2312,11 +2630,14 @@
       <c r="D105" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E105" s="3" t="s">
+      <c r="E105" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F105" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>7</v>
       </c>
@@ -2329,11 +2650,14 @@
       <c r="D106" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E106" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F106" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>7</v>
       </c>
@@ -2346,11 +2670,14 @@
       <c r="D107" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="E107" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F107" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>7</v>
       </c>
@@ -2363,11 +2690,14 @@
       <c r="D108" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E108" s="3" t="s">
+      <c r="E108" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F108" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>3</v>
       </c>
@@ -2380,900 +2710,903 @@
       <c r="D109" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E109" s="3" t="s">
+      <c r="E109" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F109" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>